<commit_message>
second olit: fix color gini
</commit_message>
<xml_diff>
--- a/ml_ai/trees/Пример создания дерева принятия решений.xlsx
+++ b/ml_ai/trees/Пример создания дерева принятия решений.xlsx
@@ -159,9 +159,6 @@
     <t>КОРНЕВОЙ СПЛИТ</t>
   </si>
   <si>
-    <t>НЕ сходится с ответами…</t>
-  </si>
-  <si>
     <t>weighted GINI INDEX Petal width</t>
   </si>
   <si>
@@ -172,6 +169,9 @@
   </si>
   <si>
     <t>На первом этапе выбираем Petal width, потому что weighted индекс джини есть наименьший</t>
+  </si>
+  <si>
+    <t>НЕ сходится с ответами…Sepal width меньше колор</t>
   </si>
 </sst>
 </file>
@@ -371,6 +371,9 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -380,24 +383,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -744,6 +734,16 @@
         <bottom/>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -755,16 +755,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:D6" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Таблица1" displayName="Таблица1" ref="A1:D6" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8">
   <autoFilter ref="A1:D6"/>
   <sortState ref="A3:D6">
     <sortCondition ref="D1:D6"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" name="Petal width" totalsRowLabel="Итог" dataDxfId="8" totalsRowDxfId="7"/>
-    <tableColumn id="2" name="Sepal width" dataDxfId="6" totalsRowDxfId="5"/>
-    <tableColumn id="3" name="Color" dataDxfId="4" totalsRowDxfId="3"/>
-    <tableColumn id="4" name="Species" dataDxfId="2" totalsRowDxfId="1"/>
+    <tableColumn id="1" name="Petal width" totalsRowLabel="Итог" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="2" name="Sepal width" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="3" name="Color" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="4" name="Species" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1059,8 +1059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1158,24 +1158,24 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="185.25" customHeight="1">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="F7" s="18" t="s">
+      <c r="B7" s="18"/>
+      <c r="F7" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="G7" s="18"/>
+      <c r="G7" s="19"/>
     </row>
     <row r="8" spans="1:7" ht="31.5">
-      <c r="A8" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="16"/>
-      <c r="F8" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="G8" s="16"/>
+      <c r="A8" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="17"/>
+      <c r="F8" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="17"/>
     </row>
     <row r="9" spans="1:7" ht="15.75">
       <c r="A9" s="5" t="s">
@@ -1345,14 +1345,14 @@
     </row>
     <row r="25" spans="1:7">
       <c r="A25" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B25" s="7">
         <f>(1/5)*B16+(4/5)*B24</f>
         <v>0.4</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G25" s="7">
         <f>1*G24</f>
@@ -1366,14 +1366,14 @@
       <c r="G26" s="8"/>
     </row>
     <row r="27" spans="1:7" ht="31.5">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="16"/>
-      <c r="F27" s="16" t="s">
+      <c r="B27" s="17"/>
+      <c r="F27" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="G27" s="16"/>
+      <c r="G27" s="17"/>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="9" t="s">
@@ -1637,14 +1637,14 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B52" s="7">
         <f>2/5 * B35 + 2/5*B51</f>
         <v>0.5</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G52" s="7">
         <f>(2/4) * G35</f>
@@ -1652,14 +1652,14 @@
       </c>
     </row>
     <row r="54" spans="1:7" ht="31.5">
-      <c r="A54" s="16" t="s">
+      <c r="A54" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B54" s="16"/>
-      <c r="F54" s="16" t="s">
+      <c r="B54" s="17"/>
+      <c r="F54" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="G54" s="16"/>
+      <c r="G54" s="17"/>
     </row>
     <row r="55" spans="1:7">
       <c r="A55" s="9" t="s">
@@ -1910,18 +1910,18 @@
     </row>
     <row r="79" spans="1:7">
       <c r="A79" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B79" s="7">
         <f>(1/5)*B62+(3/5)*B70+(1/5)*B78</f>
         <v>0.56666666666666665</v>
       </c>
       <c r="F79" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G79" s="7">
-        <f>(3/4)*G62+(3/5)*G70</f>
-        <v>0.26666666666666666</v>
+        <f>(3/4)*G62+(3/4)*G70</f>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -1931,7 +1931,7 @@
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -1939,7 +1939,7 @@
         <v>43</v>
       </c>
       <c r="F83" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1954,7 +1954,7 @@
     <mergeCell ref="F54:G54"/>
   </mergeCells>
   <conditionalFormatting sqref="D2">
-    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="4"/>
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -2009,10 +2009,10 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:2" ht="31.5">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="16" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>